<commit_message>
Update matching, match PSP data to panel
</commit_message>
<xml_diff>
--- a/figs/n_candidates.xlsx
+++ b/figs/n_candidates.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -566,7 +566,7 @@
         </is>
       </c>
       <c r="B21">
-        <v>146227</v>
+        <v>146321</v>
       </c>
     </row>
     <row r="22">
@@ -576,7 +576,7 @@
         </is>
       </c>
       <c r="B22">
-        <v>164368</v>
+        <v>164191</v>
       </c>
     </row>
     <row r="23">
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="B23">
-        <v>177870</v>
+        <v>177668</v>
       </c>
     </row>
     <row r="24">
@@ -646,7 +646,7 @@
         </is>
       </c>
       <c r="B29">
-        <v>14126</v>
+        <v>14032</v>
       </c>
     </row>
     <row r="30">
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="B30">
-        <v>15823</v>
+        <v>16000</v>
       </c>
     </row>
     <row r="31">
@@ -666,7 +666,7 @@
         </is>
       </c>
       <c r="B31">
-        <v>15453</v>
+        <v>15655</v>
       </c>
     </row>
     <row r="32">
@@ -717,6 +717,246 @@
       </c>
       <c r="B36">
         <v>16826</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Senate Election 1996</t>
+        </is>
+      </c>
+      <c r="B37">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Senate Election 1998</t>
+        </is>
+      </c>
+      <c r="B38">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Senate By-election 1999</t>
+        </is>
+      </c>
+      <c r="B39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Senate Election 2000</t>
+        </is>
+      </c>
+      <c r="B40">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Senate Election 2002</t>
+        </is>
+      </c>
+      <c r="B41">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Senate By-election 2003</t>
+        </is>
+      </c>
+      <c r="B42">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Senate By-election 2004</t>
+        </is>
+      </c>
+      <c r="B43">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Senate Election 2004</t>
+        </is>
+      </c>
+      <c r="B44">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Senate Election 2006</t>
+        </is>
+      </c>
+      <c r="B45">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Senate By-election 2007</t>
+        </is>
+      </c>
+      <c r="B46">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Senate Election 2008</t>
+        </is>
+      </c>
+      <c r="B47">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Senate Election 2010</t>
+        </is>
+      </c>
+      <c r="B48">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Senate By-election 2011</t>
+        </is>
+      </c>
+      <c r="B49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Senate Election 2012</t>
+        </is>
+      </c>
+      <c r="B50">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Senate By-election 2014</t>
+        </is>
+      </c>
+      <c r="B51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Senate Election 2014</t>
+        </is>
+      </c>
+      <c r="B52">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Senate By-election 2016</t>
+        </is>
+      </c>
+      <c r="B53">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Senate By-election 2017</t>
+        </is>
+      </c>
+      <c r="B54">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Senate By-election 2018</t>
+        </is>
+      </c>
+      <c r="B55">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Senate Election 2018</t>
+        </is>
+      </c>
+      <c r="B56">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Senate By-election 2019</t>
+        </is>
+      </c>
+      <c r="B57">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Senate By-election 2020</t>
+        </is>
+      </c>
+      <c r="B58">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Senate Election 2020</t>
+        </is>
+      </c>
+      <c r="B59">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Senate Election 2022</t>
+        </is>
+      </c>
+      <c r="B60">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Match it all together
</commit_message>
<xml_diff>
--- a/figs/n_candidates.xlsx
+++ b/figs/n_candidates.xlsx
@@ -416,7 +416,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>5059</v>
+        <v>5054</v>
       </c>
     </row>
     <row r="7">
@@ -426,7 +426,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>5906</v>
+        <v>5905</v>
       </c>
     </row>
     <row r="8">
@@ -436,7 +436,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>7540</v>
+        <v>7539</v>
       </c>
     </row>
     <row r="9">
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>5262</v>
+        <v>5258</v>
       </c>
     </row>
     <row r="10">
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="B13">
-        <v>11321</v>
+        <v>11319</v>
       </c>
     </row>
     <row r="14">
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="B14">
-        <v>11889</v>
+        <v>11888</v>
       </c>
     </row>
     <row r="15">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="B17">
-        <v>740</v>
+        <v>731</v>
       </c>
     </row>
     <row r="18">
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="B18">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="19">
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="B25">
-        <v>208997</v>
+        <v>208977</v>
       </c>
     </row>
     <row r="26">
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="B26">
-        <v>211637</v>
+        <v>211633</v>
       </c>
     </row>
     <row r="27">
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="B27">
-        <v>195882</v>
+        <v>195879</v>
       </c>
     </row>
     <row r="28">
@@ -636,7 +636,7 @@
         </is>
       </c>
       <c r="B28">
-        <v>178607</v>
+        <v>178602</v>
       </c>
     </row>
     <row r="29">
@@ -686,7 +686,7 @@
         </is>
       </c>
       <c r="B33">
-        <v>17965</v>
+        <v>17963</v>
       </c>
     </row>
     <row r="34">
@@ -696,7 +696,7 @@
         </is>
       </c>
       <c r="B34">
-        <v>22240</v>
+        <v>22235</v>
       </c>
     </row>
     <row r="35">
@@ -706,7 +706,7 @@
         </is>
       </c>
       <c r="B35">
-        <v>20623</v>
+        <v>20622</v>
       </c>
     </row>
     <row r="36">

</xml_diff>

<commit_message>
Update matching, add validations
</commit_message>
<xml_diff>
--- a/figs/n_candidates.xlsx
+++ b/figs/n_candidates.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -700,42 +700,42 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>EP 2019</t>
+          <t>EP 2004</t>
         </is>
       </c>
       <c r="B16">
-        <v>841</v>
+        <v>806</v>
       </c>
       <c r="C16">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D16">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E16">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F16">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>EP 2024</t>
+          <t>EP 2009</t>
         </is>
       </c>
       <c r="B17">
-        <v>674</v>
+        <v>708</v>
       </c>
       <c r="C17">
-        <v>245</v>
+        <v>200</v>
       </c>
       <c r="D17">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E17">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F17">
         <v>3.1</v>
@@ -744,374 +744,440 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Municipal 1994</t>
+          <t>EP 2014</t>
         </is>
       </c>
       <c r="B18">
-        <v>145611</v>
+        <v>849</v>
       </c>
       <c r="C18">
-        <v>31530</v>
+        <v>227</v>
       </c>
       <c r="D18">
-        <v>59754</v>
+        <v>21</v>
       </c>
       <c r="E18">
-        <v>10614</v>
+        <v>5</v>
       </c>
       <c r="F18">
-        <v>41</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Municipal 1998</t>
+          <t>EP 2019</t>
         </is>
       </c>
       <c r="B19">
-        <v>163664</v>
+        <v>841</v>
       </c>
       <c r="C19">
-        <v>40784</v>
+        <v>201</v>
       </c>
       <c r="D19">
-        <v>59986</v>
+        <v>21</v>
       </c>
       <c r="E19">
-        <v>12263</v>
+        <v>7</v>
       </c>
       <c r="F19">
-        <v>36.7</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Municipal 2002</t>
+          <t>EP 2024</t>
         </is>
       </c>
       <c r="B20">
-        <v>177309</v>
+        <v>674</v>
       </c>
       <c r="C20">
-        <v>48098</v>
+        <v>245</v>
       </c>
       <c r="D20">
-        <v>60001</v>
+        <v>21</v>
       </c>
       <c r="E20">
-        <v>13567</v>
+        <v>8</v>
       </c>
       <c r="F20">
-        <v>33.8</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Municipal 2006</t>
+          <t>Municipal 1994</t>
         </is>
       </c>
       <c r="B21">
-        <v>186716</v>
+        <v>145611</v>
       </c>
       <c r="C21">
-        <v>54988</v>
+        <v>31530</v>
       </c>
       <c r="D21">
-        <v>60056</v>
+        <v>59754</v>
       </c>
       <c r="E21">
-        <v>15000</v>
+        <v>10614</v>
       </c>
       <c r="F21">
-        <v>32.2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Municipal 2010</t>
+          <t>Municipal 1998</t>
         </is>
       </c>
       <c r="B22">
-        <v>208510</v>
+        <v>163664</v>
       </c>
       <c r="C22">
-        <v>65064</v>
+        <v>40784</v>
       </c>
       <c r="D22">
-        <v>59793</v>
+        <v>59986</v>
       </c>
       <c r="E22">
-        <v>15725</v>
+        <v>12263</v>
       </c>
       <c r="F22">
-        <v>28.7</v>
+        <v>36.7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Municipal 2014</t>
+          <t>Municipal 2002</t>
         </is>
       </c>
       <c r="B23">
-        <v>211295</v>
+        <v>177309</v>
       </c>
       <c r="C23">
-        <v>68091</v>
+        <v>48098</v>
       </c>
       <c r="D23">
-        <v>59573</v>
+        <v>60001</v>
       </c>
       <c r="E23">
-        <v>16129</v>
+        <v>13567</v>
       </c>
       <c r="F23">
-        <v>28.2</v>
+        <v>33.8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Municipal 2018</t>
+          <t>Municipal 2006</t>
         </is>
       </c>
       <c r="B24">
-        <v>195630</v>
+        <v>186716</v>
       </c>
       <c r="C24">
-        <v>64249</v>
+        <v>54988</v>
       </c>
       <c r="D24">
-        <v>59331</v>
+        <v>60056</v>
       </c>
       <c r="E24">
-        <v>16606</v>
+        <v>15000</v>
       </c>
       <c r="F24">
-        <v>30.3</v>
+        <v>32.2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Municipal 2022</t>
+          <t>Municipal 2010</t>
         </is>
       </c>
       <c r="B25">
-        <v>178432</v>
+        <v>208510</v>
       </c>
       <c r="C25">
-        <v>59459</v>
+        <v>65064</v>
       </c>
       <c r="D25">
-        <v>59228</v>
+        <v>59793</v>
       </c>
       <c r="E25">
-        <v>17163</v>
+        <v>15725</v>
       </c>
       <c r="F25">
-        <v>33.2</v>
+        <v>28.7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>City districts 1994</t>
+          <t>Municipal 2014</t>
         </is>
       </c>
       <c r="B26">
-        <v>13967</v>
+        <v>211295</v>
       </c>
       <c r="C26">
-        <v>4322</v>
+        <v>68091</v>
       </c>
       <c r="D26">
-        <v>2406</v>
+        <v>59573</v>
       </c>
       <c r="E26">
-        <v>527</v>
+        <v>16129</v>
       </c>
       <c r="F26">
-        <v>17.2</v>
+        <v>28.2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>City districts 1998</t>
+          <t>Municipal 2018</t>
         </is>
       </c>
       <c r="B27">
-        <v>15945</v>
+        <v>195630</v>
       </c>
       <c r="C27">
-        <v>5477</v>
+        <v>64249</v>
       </c>
       <c r="D27">
-        <v>2426</v>
+        <v>59331</v>
       </c>
       <c r="E27">
-        <v>528</v>
+        <v>16606</v>
       </c>
       <c r="F27">
-        <v>15.2</v>
+        <v>30.3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>City districts 2002</t>
+          <t>Municipal 2022</t>
         </is>
       </c>
       <c r="B28">
-        <v>15621</v>
+        <v>178432</v>
       </c>
       <c r="C28">
-        <v>5434</v>
+        <v>59459</v>
       </c>
       <c r="D28">
-        <v>2493</v>
+        <v>59228</v>
       </c>
       <c r="E28">
-        <v>615</v>
+        <v>17163</v>
       </c>
       <c r="F28">
-        <v>16</v>
+        <v>33.2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>City districts 2006</t>
+          <t>City districts 1994</t>
         </is>
       </c>
       <c r="B29">
-        <v>14948</v>
+        <v>13967</v>
       </c>
       <c r="C29">
-        <v>5421</v>
+        <v>4322</v>
       </c>
       <c r="D29">
-        <v>2519</v>
+        <v>2406</v>
       </c>
       <c r="E29">
-        <v>661</v>
+        <v>527</v>
       </c>
       <c r="F29">
-        <v>16.9</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>City districts 2010</t>
+          <t>City districts 1998</t>
         </is>
       </c>
       <c r="B30">
-        <v>17923</v>
+        <v>15945</v>
       </c>
       <c r="C30">
-        <v>6585</v>
+        <v>5477</v>
       </c>
       <c r="D30">
-        <v>2545</v>
+        <v>2426</v>
       </c>
       <c r="E30">
-        <v>711</v>
+        <v>528</v>
       </c>
       <c r="F30">
-        <v>14.2</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>City districts 2014</t>
+          <t>City districts 2002</t>
         </is>
       </c>
       <c r="B31">
-        <v>22197</v>
+        <v>15621</v>
       </c>
       <c r="C31">
-        <v>8206</v>
+        <v>5434</v>
       </c>
       <c r="D31">
-        <v>2548</v>
+        <v>2493</v>
       </c>
       <c r="E31">
-        <v>730</v>
+        <v>615</v>
       </c>
       <c r="F31">
-        <v>11.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>City districts 2018</t>
+          <t>City districts 2006</t>
         </is>
       </c>
       <c r="B32">
-        <v>20531</v>
+        <v>14948</v>
       </c>
       <c r="C32">
-        <v>7828</v>
+        <v>5421</v>
       </c>
       <c r="D32">
-        <v>2561</v>
+        <v>2519</v>
       </c>
       <c r="E32">
-        <v>729</v>
+        <v>661</v>
       </c>
       <c r="F32">
-        <v>12.5</v>
+        <v>16.9</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>City districts 2022</t>
+          <t>City districts 2010</t>
         </is>
       </c>
       <c r="B33">
-        <v>16791</v>
+        <v>17923</v>
       </c>
       <c r="C33">
-        <v>6648</v>
+        <v>6585</v>
       </c>
       <c r="D33">
-        <v>2552</v>
+        <v>2545</v>
       </c>
       <c r="E33">
-        <v>756</v>
+        <v>711</v>
       </c>
       <c r="F33">
-        <v>15.2</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>City districts 2014</t>
+        </is>
+      </c>
+      <c r="B34">
+        <v>22197</v>
+      </c>
+      <c r="C34">
+        <v>8206</v>
+      </c>
+      <c r="D34">
+        <v>2548</v>
+      </c>
+      <c r="E34">
+        <v>730</v>
+      </c>
+      <c r="F34">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>City districts 2018</t>
+        </is>
+      </c>
+      <c r="B35">
+        <v>20531</v>
+      </c>
+      <c r="C35">
+        <v>7828</v>
+      </c>
+      <c r="D35">
+        <v>2561</v>
+      </c>
+      <c r="E35">
+        <v>729</v>
+      </c>
+      <c r="F35">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>City districts 2022</t>
+        </is>
+      </c>
+      <c r="B36">
+        <v>16791</v>
+      </c>
+      <c r="C36">
+        <v>6648</v>
+      </c>
+      <c r="D36">
+        <v>2552</v>
+      </c>
+      <c r="E36">
+        <v>756</v>
+      </c>
+      <c r="F36">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>Senate By-elections</t>
         </is>
       </c>
-      <c r="B34">
+      <c r="B37">
         <v>3343</v>
       </c>
-      <c r="C34">
+      <c r="C37">
         <v>539</v>
       </c>
-      <c r="D34">
+      <c r="D37">
         <v>447</v>
       </c>
-      <c r="E34">
+      <c r="E37">
         <v>70</v>
       </c>
-      <c r="F34">
+      <c r="F37">
         <v>13.4</v>
       </c>
     </row>

</xml_diff>